<commit_message>
removed deatils in hr.xlsx
</commit_message>
<xml_diff>
--- a/src/main/resources/hr.xlsx
+++ b/src/main/resources/hr.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chand\Desktop\Automatic-Email-Sender-Hr\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B192B387-A021-4743-A7D3-7B0E560F1F3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C05E30EC-029D-4289-A28A-9932E12FC44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>SNo</t>
   </si>
@@ -35,18 +35,6 @@
   </si>
   <si>
     <t>Company</t>
-  </si>
-  <si>
-    <t>Associate Vice President Human Resources</t>
-  </si>
-  <si>
-    <t>Chandu</t>
-  </si>
-  <si>
-    <t>chanduraparthi1@gmail.com</t>
-  </si>
-  <si>
-    <t>XSS</t>
   </si>
 </sst>
 </file>
@@ -356,7 +344,7 @@
   <dimension ref="A1:E1843"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -379,21 +367,11 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
@@ -13283,9 +13261,6 @@
       <c r="E1843" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{F55AAD6A-7889-4CF0-9B79-DDD38FB7CB77}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>